<commit_message>
ebi-ait/dcp-ingest-central#650: removed schemas tab from spreadsheet
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Documents/GitHub_Issues/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaider/hca/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C30C3D0-8F58-2A43-9023-2E9338C3A6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9DC217-D4DC-9E42-891F-1C450E2F0AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24000" yWindow="3420" windowWidth="24600" windowHeight="22840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-2280" windowWidth="51200" windowHeight="28800" firstSheet="16" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -42,14 +42,13 @@
     <sheet name="Imaging protocol - Channel" sheetId="25" r:id="rId27"/>
     <sheet name="Imaging protocol - Probe" sheetId="26" r:id="rId28"/>
     <sheet name="Familial relationship" sheetId="27" r:id="rId29"/>
-    <sheet name="Schemas" sheetId="28" r:id="rId30"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="1517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1490">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4339,87 +4338,6 @@
   </si>
   <si>
     <t>donor_organism.familial_relationships.sibling</t>
-  </si>
-  <si>
-    <t>Schemas</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/sequencing/10.1.0/sequencing_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/sequencing/6.2.0/library_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/imaging/11.2.0/imaging_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/imaging/2.2.0/imaging_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/3.2.0/ipsc_induction_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/3.1.0/enrichment_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/6.2.0/dissociation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/2.2.0/differentiation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/9.2.0/collection_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/biomaterial_collection/2.1.0/aggregate_generation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/analysis/9.1.0/analysis_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/protocol/7.1.0/protocol</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/project/14.1.0/project</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/process/analysis/11.1.0/analysis_process</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/process/9.2.0/process</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/file/2.2.0/supplementary_file</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/file/9.2.0/sequence_file</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/file/3.2.0/reference_file</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/file/2.2.0/image_file</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/file/6.2.0/analysis_file</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/10.4.0/specimen_from_organism</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/11.3.0/organoid</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/3.3.0/imaged_specimen</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/15.5.0/donor_organism</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/13.3.0/cell_suspension</t>
-  </si>
-  <si>
-    <t>https://schema.staging.data.humancellatlas.org/type/biomaterial/14.5.0/cell_line</t>
   </si>
   <si>
     <t>EGA Study/Dataset Accession(s)</t>
@@ -4606,7 +4524,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4629,13 +4547,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4668,14 +4579,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4684,18 +4591,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5076,11 +4981,11 @@
       <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>1457</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>1458</v>
+      <c r="J1" s="4" t="s">
+        <v>1430</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1431</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>579</v>
@@ -5115,13 +5020,13 @@
         <v>34</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1459</v>
+        <v>1432</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>1460</v>
+        <v>1433</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>1511</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
@@ -5153,13 +5058,13 @@
         <v>35</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1461</v>
+        <v>1434</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>1462</v>
+        <v>1435</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>1512</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -5191,13 +5096,13 @@
         <v>36</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1463</v>
+        <v>1436</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1464</v>
+        <v>1437</v>
       </c>
       <c r="L4" t="s">
-        <v>1510</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -10601,88 +10506,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>815</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>819</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>1489</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="4" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>1488</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>1490</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>1491</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>863</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>865</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>1492</v>
-      </c>
-      <c r="S1" s="5" t="s">
+      <c r="R1" s="4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>1493</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>1494</v>
-      </c>
-      <c r="Y1" s="5" t="s">
+      <c r="W1" s="4" t="s">
+        <v>1466</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>1467</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>1495</v>
-      </c>
-      <c r="AA1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>1468</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>369</v>
       </c>
     </row>
@@ -10694,7 +10599,7 @@
         <v>816</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1496</v>
+        <v>1469</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>74</v>
@@ -10706,10 +10611,10 @@
         <v>829</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1504</v>
+        <v>1477</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>1506</v>
+        <v>1479</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>492</v>
@@ -10790,10 +10695,10 @@
         <v>830</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1505</v>
+        <v>1478</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1507</v>
+        <v>1480</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>493</v>
@@ -10844,36 +10749,36 @@
     </row>
     <row r="4" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>1497</v>
+        <v>1470</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1499</v>
+        <v>1471</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1472</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1500</v>
+        <v>1473</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1501</v>
+        <v>1474</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1502</v>
+        <v>1475</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1508</v>
+        <v>1481</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>1503</v>
+        <v>1476</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1478</v>
-      </c>
-      <c r="J4" s="6" t="s">
+        <v>1451</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>864</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -10929,11 +10834,11 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10941,7 +10846,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -10961,396 +10866,396 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
     </row>
     <row r="22" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
     </row>
     <row r="23" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
     </row>
     <row r="24" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
     </row>
     <row r="25" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
     </row>
     <row r="26" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
     </row>
     <row r="28" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
     </row>
     <row r="29" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
     </row>
     <row r="30" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
     </row>
     <row r="31" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
     </row>
     <row r="32" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
     </row>
     <row r="33" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
     </row>
     <row r="34" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
     </row>
     <row r="35" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
     </row>
     <row r="36" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
     </row>
     <row r="37" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
     </row>
     <row r="38" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
     </row>
     <row r="39" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
     </row>
     <row r="40" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
     </row>
     <row r="41" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
     </row>
     <row r="42" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
     </row>
     <row r="43" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
     </row>
     <row r="44" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
     </row>
     <row r="45" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
     </row>
     <row r="46" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
     </row>
     <row r="47" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
     </row>
     <row r="48" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
     </row>
     <row r="49" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
     </row>
     <row r="50" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
     </row>
     <row r="51" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
     </row>
     <row r="52" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
     </row>
     <row r="53" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
     </row>
     <row r="54" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q54" s="8"/>
-      <c r="R54" s="8"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
     </row>
     <row r="55" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
     </row>
     <row r="56" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
     </row>
     <row r="57" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
     </row>
     <row r="58" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q58" s="8"/>
-      <c r="R58" s="8"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
     </row>
     <row r="59" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q59" s="8"/>
-      <c r="R59" s="8"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
     </row>
     <row r="60" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
     </row>
     <row r="61" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q61" s="8"/>
-      <c r="R61" s="8"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
     </row>
     <row r="62" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
     </row>
     <row r="63" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q63" s="8"/>
-      <c r="R63" s="8"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
     </row>
     <row r="64" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q64" s="8"/>
-      <c r="R64" s="8"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
     </row>
     <row r="65" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q65" s="8"/>
-      <c r="R65" s="8"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
     </row>
     <row r="66" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q66" s="8"/>
-      <c r="R66" s="8"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
     </row>
     <row r="67" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q67" s="8"/>
-      <c r="R67" s="8"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="7"/>
     </row>
     <row r="68" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q68" s="8"/>
-      <c r="R68" s="8"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
     </row>
     <row r="69" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q69" s="8"/>
-      <c r="R69" s="8"/>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7"/>
     </row>
     <row r="70" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q70" s="8"/>
-      <c r="R70" s="8"/>
+      <c r="Q70" s="7"/>
+      <c r="R70" s="7"/>
     </row>
     <row r="71" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q71" s="8"/>
-      <c r="R71" s="8"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
     </row>
     <row r="72" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q72" s="8"/>
-      <c r="R72" s="8"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
     </row>
     <row r="73" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q73" s="8"/>
-      <c r="R73" s="8"/>
+      <c r="Q73" s="7"/>
+      <c r="R73" s="7"/>
     </row>
     <row r="74" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q74" s="8"/>
-      <c r="R74" s="8"/>
+      <c r="Q74" s="7"/>
+      <c r="R74" s="7"/>
     </row>
     <row r="75" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q75" s="8"/>
-      <c r="R75" s="8"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7"/>
     </row>
     <row r="76" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q76" s="8"/>
-      <c r="R76" s="8"/>
+      <c r="Q76" s="7"/>
+      <c r="R76" s="7"/>
     </row>
     <row r="77" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q77" s="8"/>
-      <c r="R77" s="8"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="7"/>
     </row>
     <row r="78" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q78" s="8"/>
-      <c r="R78" s="8"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
     </row>
     <row r="79" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q79" s="8"/>
-      <c r="R79" s="8"/>
+      <c r="Q79" s="7"/>
+      <c r="R79" s="7"/>
     </row>
     <row r="80" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q80" s="8"/>
-      <c r="R80" s="8"/>
+      <c r="Q80" s="7"/>
+      <c r="R80" s="7"/>
     </row>
     <row r="81" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q81" s="8"/>
-      <c r="R81" s="8"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
     </row>
     <row r="82" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q82" s="8"/>
-      <c r="R82" s="8"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
     </row>
     <row r="83" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q83" s="8"/>
-      <c r="R83" s="8"/>
+      <c r="Q83" s="7"/>
+      <c r="R83" s="7"/>
     </row>
     <row r="84" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q84" s="8"/>
-      <c r="R84" s="8"/>
+      <c r="Q84" s="7"/>
+      <c r="R84" s="7"/>
     </row>
     <row r="85" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q85" s="8"/>
-      <c r="R85" s="8"/>
+      <c r="Q85" s="7"/>
+      <c r="R85" s="7"/>
     </row>
     <row r="86" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q86" s="8"/>
-      <c r="R86" s="8"/>
+      <c r="Q86" s="7"/>
+      <c r="R86" s="7"/>
     </row>
     <row r="87" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q87" s="8"/>
-      <c r="R87" s="8"/>
+      <c r="Q87" s="7"/>
+      <c r="R87" s="7"/>
     </row>
     <row r="88" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q88" s="8"/>
-      <c r="R88" s="8"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
     </row>
     <row r="89" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
     </row>
     <row r="90" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
     </row>
     <row r="91" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q91" s="8"/>
-      <c r="R91" s="8"/>
+      <c r="Q91" s="7"/>
+      <c r="R91" s="7"/>
     </row>
     <row r="92" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8"/>
+      <c r="Q92" s="7"/>
+      <c r="R92" s="7"/>
     </row>
     <row r="93" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8"/>
+      <c r="Q93" s="7"/>
+      <c r="R93" s="7"/>
     </row>
     <row r="94" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q94" s="8"/>
-      <c r="R94" s="8"/>
+      <c r="Q94" s="7"/>
+      <c r="R94" s="7"/>
     </row>
     <row r="95" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
+      <c r="Q95" s="7"/>
+      <c r="R95" s="7"/>
     </row>
     <row r="96" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q96" s="8"/>
-      <c r="R96" s="8"/>
+      <c r="Q96" s="7"/>
+      <c r="R96" s="7"/>
     </row>
     <row r="97" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q97" s="8"/>
-      <c r="R97" s="8"/>
+      <c r="Q97" s="7"/>
+      <c r="R97" s="7"/>
     </row>
     <row r="98" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q98" s="8"/>
-      <c r="R98" s="8"/>
+      <c r="Q98" s="7"/>
+      <c r="R98" s="7"/>
     </row>
     <row r="99" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q99" s="8"/>
-      <c r="R99" s="8"/>
+      <c r="Q99" s="7"/>
+      <c r="R99" s="7"/>
     </row>
     <row r="100" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q100" s="8"/>
-      <c r="R100" s="8"/>
+      <c r="Q100" s="7"/>
+      <c r="R100" s="7"/>
     </row>
     <row r="101" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q101" s="8"/>
-      <c r="R101" s="8"/>
+      <c r="Q101" s="7"/>
+      <c r="R101" s="7"/>
     </row>
     <row r="102" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q102" s="8"/>
-      <c r="R102" s="8"/>
+      <c r="Q102" s="7"/>
+      <c r="R102" s="7"/>
     </row>
     <row r="103" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q103" s="8"/>
-      <c r="R103" s="8"/>
+      <c r="Q103" s="7"/>
+      <c r="R103" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11384,43 +11289,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1467</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>885</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>1468</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1469</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>1470</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>1471</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>1472</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>1473</v>
-      </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="F1" s="4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>1444</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1445</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -11443,10 +11348,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>1474</v>
+        <v>1447</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>1475</v>
+        <v>1448</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -11470,10 +11375,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>1476</v>
+        <v>1449</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>1477</v>
+        <v>1450</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -11482,37 +11387,37 @@
     </row>
     <row r="4" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>1478</v>
+        <v>1451</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1479</v>
+        <v>1452</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1480</v>
+        <v>1453</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1481</v>
+        <v>1454</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>1482</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>1483</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>1484</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>1485</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>1486</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>1509</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>1487</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -12045,7 +11950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12112,7 +12017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -12141,7 +12046,7 @@
         <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1513</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
@@ -12161,7 +12066,7 @@
         <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1514</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -12181,7 +12086,7 @@
         <v>102</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1515</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -12201,7 +12106,7 @@
         <v>103</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1516</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -12215,182 +12120,6 @@
       <c r="F5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:A27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>1435</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>1439</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>1449</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>1451</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>1452</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>1453</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-1B00-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-1B00-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-1B00-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-1B00-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-1B00-000005000000}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-1B00-000006000000}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-1B00-000007000000}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-1B00-000008000000}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-1B00-000009000000}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-1B00-00000A000000}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-1B00-00000B000000}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-1B00-00000C000000}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-1B00-00000D000000}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-1B00-00000E000000}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-1B00-00000F000000}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-1B00-000010000000}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-1B00-000011000000}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-1B00-000012000000}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-1B00-000013000000}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-1B00-000014000000}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-1B00-000015000000}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-1B00-000016000000}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-1B00-000017000000}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-1B00-000018000000}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-1B00-000019000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add analysis_protocol.text and analysis_protocol.computational_method descriptions back to spreadsheet
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A032942-648D-D248-A5FC-4B9A39D3055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F13E06-52A2-A843-9CCA-8257E86C22AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33100" windowHeight="21460" firstSheet="17" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3038" uniqueCount="1566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="1570">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4748,6 +4748,18 @@
   </si>
   <si>
     <t>sequence_file.file_core.file_source</t>
+  </si>
+  <si>
+    <t>The type of protocol.</t>
+  </si>
+  <si>
+    <t>For example: raw matrix generation; processed matrix generation</t>
+  </si>
+  <si>
+    <t>A URI to a versioned workflow and versioned execution environment in a GA4GH-compliant repository.</t>
+  </si>
+  <si>
+    <t>For example: SmartSeq2SingleCell; 10x</t>
   </si>
 </sst>
 </file>
@@ -5198,7 +5210,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6817,7 +6829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -8608,7 +8620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8616,9 +8630,11 @@
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="12" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -10824,7 +10840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11006,7 +11024,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>862</v>
       </c>
@@ -11093,8 +11111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B387E90-E3CD-9746-8D43-32F9BE05CBD7}">
   <dimension ref="A1:AB103"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11883,8 +11901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11959,10 +11977,18 @@
       <c r="E2" s="2" t="s">
         <v>882</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1568</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>1443</v>
       </c>
@@ -11986,10 +12012,18 @@
       <c r="E3" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>1567</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1569</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>1445</v>
       </c>
@@ -12293,7 +12327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12745,7 +12781,7 @@
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12969,8 +13005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BY5"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AE1048576"/>
+    <sheetView topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BU4" sqref="BU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated with genome and patch version for analysis files
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F13E06-52A2-A843-9CCA-8257E86C22AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AFB9F36-2986-AB4F-9168-69691A49C3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33100" windowHeight="21460" firstSheet="17" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33100" windowHeight="21460" firstSheet="21" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1578">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4760,6 +4760,30 @@
   </si>
   <si>
     <t>For example: SmartSeq2SingleCell; 10x</t>
+  </si>
+  <si>
+    <t>analysis_file.genome_assembly_version</t>
+  </si>
+  <si>
+    <t>analysis_file.genome_patch_version</t>
+  </si>
+  <si>
+    <t>Name of the genome assembly used to generate this file.</t>
+  </si>
+  <si>
+    <t>Patch version of the genome assembly used to generate this file.</t>
+  </si>
+  <si>
+    <t>GENOME VERSION (Required)</t>
+  </si>
+  <si>
+    <t>PATCH VERSION</t>
+  </si>
+  <si>
+    <t>Please use the name as defined in the Genome Reference Consortium (https://www.ncbi.nlm.nih.gov/grc). Should be one of: GRCh38, GRCh37, GRCm39, GRCm38, GRCm37, Not Applicable</t>
+  </si>
+  <si>
+    <t>For example: p11; p14</t>
   </si>
 </sst>
 </file>
@@ -8675,7 +8699,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>488</v>
       </c>
@@ -8713,7 +8737,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>489</v>
       </c>
@@ -11109,10 +11133,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B387E90-E3CD-9746-8D43-32F9BE05CBD7}">
-  <dimension ref="A1:AB103"/>
+  <dimension ref="A1:AD103"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11124,23 +11148,26 @@
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="7" max="7" width="53.5" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="17" width="18.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" customWidth="1"/>
-    <col min="19" max="20" width="8.83203125" customWidth="1"/>
-    <col min="21" max="21" width="18.6640625" customWidth="1"/>
-    <col min="22" max="22" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.6640625" customWidth="1"/>
-    <col min="25" max="25" width="30.6640625" customWidth="1"/>
-    <col min="26" max="26" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.83203125" customWidth="1"/>
+    <col min="9" max="10" width="39" customWidth="1"/>
+    <col min="11" max="11" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="55" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1"/>
+    <col min="21" max="22" width="8.83203125" customWidth="1"/>
+    <col min="23" max="23" width="18.6640625" customWidth="1"/>
+    <col min="24" max="24" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.6640625" customWidth="1"/>
+    <col min="27" max="27" width="30.6640625" customWidth="1"/>
+    <col min="28" max="28" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.83203125" customWidth="1"/>
+    <col min="30" max="30" width="18.5" customWidth="1"/>
+    <col min="31" max="31" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>807</v>
       </c>
@@ -11166,67 +11193,73 @@
         <v>1459</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>1574</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1575</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1460</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1461</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1462</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1463</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1464</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>808</v>
       </c>
@@ -11252,67 +11285,73 @@
         <v>1475</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>488</v>
+        <v>1572</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>117</v>
+        <v>1573</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>488</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>809</v>
       </c>
@@ -11336,53 +11375,59 @@
         <v>1476</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>1576</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1577</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2"/>
+      <c r="X3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1466</v>
       </c>
@@ -11408,67 +11453,73 @@
         <v>1472</v>
       </c>
       <c r="I4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="K4" t="s">
         <v>1447</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>862</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>321</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>324</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>327</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>331</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>335</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>339</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>342</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>346</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>348</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>350</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>352</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>356</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>359</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
         <v>361</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>365</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AD4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -11481,9 +11532,9 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -11499,398 +11550,400 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-    </row>
-    <row r="18" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-    </row>
-    <row r="20" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-    </row>
-    <row r="23" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-    </row>
-    <row r="24" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-    </row>
-    <row r="25" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-    </row>
-    <row r="26" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-    </row>
-    <row r="27" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-    </row>
-    <row r="28" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-    </row>
-    <row r="29" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-    </row>
-    <row r="30" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-    </row>
-    <row r="31" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-    </row>
-    <row r="32" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-    </row>
-    <row r="33" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-    </row>
-    <row r="34" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-    </row>
-    <row r="35" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-    </row>
-    <row r="36" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-    </row>
-    <row r="37" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-    </row>
-    <row r="38" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-    </row>
-    <row r="39" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-    </row>
-    <row r="40" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-    </row>
-    <row r="41" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-    </row>
-    <row r="42" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-    </row>
-    <row r="43" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-    </row>
-    <row r="44" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-    </row>
-    <row r="45" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-    </row>
-    <row r="46" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-    </row>
-    <row r="47" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
-    </row>
-    <row r="48" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
-    </row>
-    <row r="49" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-    </row>
-    <row r="50" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
-    </row>
-    <row r="51" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-    </row>
-    <row r="52" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-    </row>
-    <row r="53" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-    </row>
-    <row r="54" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-    </row>
-    <row r="55" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-    </row>
-    <row r="56" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
-    </row>
-    <row r="57" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
-    </row>
-    <row r="58" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
-    </row>
-    <row r="59" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q59" s="6"/>
-      <c r="R59" s="6"/>
-    </row>
-    <row r="60" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q60" s="6"/>
-      <c r="R60" s="6"/>
-    </row>
-    <row r="61" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
-    </row>
-    <row r="62" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
-    </row>
-    <row r="63" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
-    </row>
-    <row r="64" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q64" s="6"/>
-      <c r="R64" s="6"/>
-    </row>
-    <row r="65" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q65" s="6"/>
-      <c r="R65" s="6"/>
-    </row>
-    <row r="66" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
-    </row>
-    <row r="67" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q67" s="6"/>
-      <c r="R67" s="6"/>
-    </row>
-    <row r="68" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q68" s="6"/>
-      <c r="R68" s="6"/>
-    </row>
-    <row r="69" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-    </row>
-    <row r="70" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
-    </row>
-    <row r="71" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q71" s="6"/>
-      <c r="R71" s="6"/>
-    </row>
-    <row r="72" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q72" s="6"/>
-      <c r="R72" s="6"/>
-    </row>
-    <row r="73" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q73" s="6"/>
-      <c r="R73" s="6"/>
-    </row>
-    <row r="74" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q74" s="6"/>
-      <c r="R74" s="6"/>
-    </row>
-    <row r="75" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
-    </row>
-    <row r="76" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
-    </row>
-    <row r="77" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-    </row>
-    <row r="78" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-    </row>
-    <row r="79" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-    </row>
-    <row r="80" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
-    </row>
-    <row r="81" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
-    </row>
-    <row r="82" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
-    </row>
-    <row r="83" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q83" s="6"/>
-      <c r="R83" s="6"/>
-    </row>
-    <row r="84" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q84" s="6"/>
-      <c r="R84" s="6"/>
-    </row>
-    <row r="85" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q85" s="6"/>
-      <c r="R85" s="6"/>
-    </row>
-    <row r="86" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q86" s="6"/>
-      <c r="R86" s="6"/>
-    </row>
-    <row r="87" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6"/>
-    </row>
-    <row r="88" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q88" s="6"/>
-      <c r="R88" s="6"/>
-    </row>
-    <row r="89" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q89" s="6"/>
-      <c r="R89" s="6"/>
-    </row>
-    <row r="90" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q90" s="6"/>
-      <c r="R90" s="6"/>
-    </row>
-    <row r="91" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q91" s="6"/>
-      <c r="R91" s="6"/>
-    </row>
-    <row r="92" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q92" s="6"/>
-      <c r="R92" s="6"/>
-    </row>
-    <row r="93" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q93" s="6"/>
-      <c r="R93" s="6"/>
-    </row>
-    <row r="94" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q94" s="6"/>
-      <c r="R94" s="6"/>
-    </row>
-    <row r="95" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q95" s="6"/>
-      <c r="R95" s="6"/>
-    </row>
-    <row r="96" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q96" s="6"/>
-      <c r="R96" s="6"/>
-    </row>
-    <row r="97" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q97" s="6"/>
-      <c r="R97" s="6"/>
-    </row>
-    <row r="98" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q98" s="6"/>
-      <c r="R98" s="6"/>
-    </row>
-    <row r="99" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q99" s="6"/>
-      <c r="R99" s="6"/>
-    </row>
-    <row r="100" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q100" s="6"/>
-      <c r="R100" s="6"/>
-    </row>
-    <row r="101" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q101" s="6"/>
-      <c r="R101" s="6"/>
-    </row>
-    <row r="102" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
-    </row>
-    <row r="103" spans="17:18" x14ac:dyDescent="0.2">
-      <c r="Q103" s="6"/>
-      <c r="R103" s="6"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+    </row>
+    <row r="25" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+    </row>
+    <row r="27" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+    </row>
+    <row r="30" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+    </row>
+    <row r="35" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+    </row>
+    <row r="36" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+    </row>
+    <row r="37" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+    </row>
+    <row r="38" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+    </row>
+    <row r="39" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+    </row>
+    <row r="40" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+    </row>
+    <row r="41" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+    </row>
+    <row r="42" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+    </row>
+    <row r="43" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+    </row>
+    <row r="44" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+    </row>
+    <row r="45" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+    </row>
+    <row r="46" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+    </row>
+    <row r="47" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
+    </row>
+    <row r="48" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S48" s="6"/>
+      <c r="T48" s="6"/>
+    </row>
+    <row r="49" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S49" s="6"/>
+      <c r="T49" s="6"/>
+    </row>
+    <row r="50" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S50" s="6"/>
+      <c r="T50" s="6"/>
+    </row>
+    <row r="51" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
+    </row>
+    <row r="52" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+    </row>
+    <row r="53" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+    </row>
+    <row r="54" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+    </row>
+    <row r="55" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+    </row>
+    <row r="56" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+    </row>
+    <row r="57" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+    </row>
+    <row r="58" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+    </row>
+    <row r="59" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+    </row>
+    <row r="60" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+    </row>
+    <row r="61" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+    </row>
+    <row r="62" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
+    </row>
+    <row r="63" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S63" s="6"/>
+      <c r="T63" s="6"/>
+    </row>
+    <row r="64" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+    </row>
+    <row r="65" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+    </row>
+    <row r="66" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+    </row>
+    <row r="67" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+    </row>
+    <row r="68" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+    </row>
+    <row r="69" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+    </row>
+    <row r="70" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S70" s="6"/>
+      <c r="T70" s="6"/>
+    </row>
+    <row r="71" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S71" s="6"/>
+      <c r="T71" s="6"/>
+    </row>
+    <row r="72" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S72" s="6"/>
+      <c r="T72" s="6"/>
+    </row>
+    <row r="73" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S73" s="6"/>
+      <c r="T73" s="6"/>
+    </row>
+    <row r="74" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S74" s="6"/>
+      <c r="T74" s="6"/>
+    </row>
+    <row r="75" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S75" s="6"/>
+      <c r="T75" s="6"/>
+    </row>
+    <row r="76" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S76" s="6"/>
+      <c r="T76" s="6"/>
+    </row>
+    <row r="77" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S77" s="6"/>
+      <c r="T77" s="6"/>
+    </row>
+    <row r="78" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S78" s="6"/>
+      <c r="T78" s="6"/>
+    </row>
+    <row r="79" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S79" s="6"/>
+      <c r="T79" s="6"/>
+    </row>
+    <row r="80" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S80" s="6"/>
+      <c r="T80" s="6"/>
+    </row>
+    <row r="81" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S81" s="6"/>
+      <c r="T81" s="6"/>
+    </row>
+    <row r="82" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S82" s="6"/>
+      <c r="T82" s="6"/>
+    </row>
+    <row r="83" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S83" s="6"/>
+      <c r="T83" s="6"/>
+    </row>
+    <row r="84" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S84" s="6"/>
+      <c r="T84" s="6"/>
+    </row>
+    <row r="85" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S85" s="6"/>
+      <c r="T85" s="6"/>
+    </row>
+    <row r="86" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S86" s="6"/>
+      <c r="T86" s="6"/>
+    </row>
+    <row r="87" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S87" s="6"/>
+      <c r="T87" s="6"/>
+    </row>
+    <row r="88" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S88" s="6"/>
+      <c r="T88" s="6"/>
+    </row>
+    <row r="89" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S89" s="6"/>
+      <c r="T89" s="6"/>
+    </row>
+    <row r="90" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S90" s="6"/>
+      <c r="T90" s="6"/>
+    </row>
+    <row r="91" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S91" s="6"/>
+      <c r="T91" s="6"/>
+    </row>
+    <row r="92" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S92" s="6"/>
+      <c r="T92" s="6"/>
+    </row>
+    <row r="93" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S93" s="6"/>
+      <c r="T93" s="6"/>
+    </row>
+    <row r="94" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S94" s="6"/>
+      <c r="T94" s="6"/>
+    </row>
+    <row r="95" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S95" s="6"/>
+      <c r="T95" s="6"/>
+    </row>
+    <row r="96" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S96" s="6"/>
+      <c r="T96" s="6"/>
+    </row>
+    <row r="97" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S97" s="6"/>
+      <c r="T97" s="6"/>
+    </row>
+    <row r="98" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S98" s="6"/>
+      <c r="T98" s="6"/>
+    </row>
+    <row r="99" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S99" s="6"/>
+      <c r="T99" s="6"/>
+    </row>
+    <row r="100" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S100" s="6"/>
+      <c r="T100" s="6"/>
+    </row>
+    <row r="101" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S101" s="6"/>
+      <c r="T101" s="6"/>
+    </row>
+    <row r="102" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S102" s="6"/>
+      <c r="T102" s="6"/>
+    </row>
+    <row r="103" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S103" s="6"/>
+      <c r="T103" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11901,7 +11954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add specimen field adjacent_diseases
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idazucchi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AFB9F36-2986-AB4F-9168-69691A49C3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB25997-AA76-DB4B-9385-0AD0F9D8E6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33100" windowHeight="21460" firstSheet="21" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4580" yWindow="-21600" windowWidth="38400" windowHeight="21600" firstSheet="20" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3066" uniqueCount="1586">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4684,9 +4684,6 @@
     <t>https://schema.humancellatlas.org/type/file/6.5.0/analysis_file</t>
   </si>
   <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/10.5.0/specimen_from_organism</t>
-  </si>
-  <si>
     <t>https://schema.humancellatlas.org/type/biomaterial/11.3.0/organoid</t>
   </si>
   <si>
@@ -4784,6 +4781,33 @@
   </si>
   <si>
     <t>For example: p11; p14</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.adjacent_diseases.text</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.adjacent_diseases.ontology</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.adjacent_diseases.ontology_label</t>
+  </si>
+  <si>
+    <t>ADJACENT DISEASE(S)</t>
+  </si>
+  <si>
+    <t>ADJACENT DISEASE(S)) ONTOLOGY ID</t>
+  </si>
+  <si>
+    <t>ADJACENT DISEASE(S) ONTOLOGY LABEL ONTOLOGY ID</t>
+  </si>
+  <si>
+    <t>Short description of the disease(s) adjacent to the specimen's collection site (e.g. breast cancer).</t>
+  </si>
+  <si>
+    <t>If a healthy specimen is sampled from a site adjacent to diseased tissue, enter that tissue's disease here. If no diseased tissue is adjacent to the specimen, leave blank. For example: type 2 diabetes mellitus; normal; hepatic steatosis</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/10.6.0/specimen_from_organism</t>
   </si>
 </sst>
 </file>
@@ -5233,8 +5257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5361,7 +5385,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5424,9 +5448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AU1" sqref="AU1:AV1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6853,8 +6875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7152,7 +7174,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>832</v>
       </c>
@@ -7172,7 +7194,7 @@
         <v>837</v>
       </c>
       <c r="G4" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="H4" t="s">
         <v>841</v>
@@ -7858,8 +7880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2F1E06-C83F-9240-A431-D0EEE8C93825}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7904,7 +7926,7 @@
         <v>1507</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>895</v>
@@ -7954,16 +7976,16 @@
         <v>886</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>463</v>
@@ -7984,10 +8006,10 @@
         <v>483</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>78</v>
@@ -8009,13 +8031,13 @@
         <v>887</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>938</v>
@@ -8039,16 +8061,16 @@
         <v>484</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1511</v>
       </c>
@@ -8080,22 +8102,22 @@
         <v>1520</v>
       </c>
       <c r="K4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="L4" t="s">
         <v>1557</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>1558</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>1559</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>1560</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>1561</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1562</v>
       </c>
       <c r="Q4" t="s">
         <v>1521</v>
@@ -8364,9 +8386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9772,9 +9792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10864,8 +10882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11048,7 +11066,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>862</v>
       </c>
@@ -11135,14 +11153,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B387E90-E3CD-9746-8D43-32F9BE05CBD7}">
   <dimension ref="A1:AD103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="1" max="2" width="38.6640625" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="58.83203125" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
@@ -11193,10 +11210,10 @@
         <v>1459</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>1573</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1574</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1575</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1460</v>
@@ -11285,10 +11302,10 @@
         <v>1475</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>1571</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>1572</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>1573</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>488</v>
@@ -11375,10 +11392,10 @@
         <v>1476</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>1575</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>1576</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1577</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>489</v>
@@ -11427,7 +11444,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1466</v>
       </c>
@@ -11453,10 +11470,10 @@
         <v>1472</v>
       </c>
       <c r="I4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="J4" t="s">
         <v>1570</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1571</v>
       </c>
       <c r="K4" t="s">
         <v>1447</v>
@@ -11954,8 +11971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12031,7 +12048,7 @@
         <v>882</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>74</v>
@@ -12040,7 +12057,7 @@
         <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>1443</v>
@@ -12066,7 +12083,7 @@
         <v>883</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>358</v>
@@ -12075,7 +12092,7 @@
         <v>355</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>1445</v>
@@ -12088,7 +12105,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1447</v>
       </c>
@@ -12380,8 +12397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12656,7 +12673,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12727,7 +12744,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -12833,8 +12850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12946,37 +12963,37 @@
     </row>
     <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>1544</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
   </sheetData>
@@ -13058,8 +13075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BY5"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BU4" sqref="BU4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14110,10 +14127,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:BH5"/>
+  <dimension ref="A1:BK5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:U1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14129,26 +14146,28 @@
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="25.6640625" customWidth="1"/>
     <col min="20" max="21" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="22" max="32" width="25.6640625" customWidth="1"/>
-    <col min="33" max="34" width="0" hidden="1" customWidth="1"/>
-    <col min="35" max="36" width="25.6640625" customWidth="1"/>
-    <col min="37" max="37" width="32.6640625" customWidth="1"/>
-    <col min="38" max="38" width="35.6640625" customWidth="1"/>
-    <col min="39" max="39" width="33.6640625" customWidth="1"/>
-    <col min="40" max="40" width="37.6640625" customWidth="1"/>
-    <col min="41" max="41" width="32.6640625" customWidth="1"/>
-    <col min="42" max="42" width="26.6640625" customWidth="1"/>
-    <col min="43" max="43" width="34.6640625" customWidth="1"/>
-    <col min="44" max="44" width="33.6640625" customWidth="1"/>
-    <col min="45" max="53" width="25.6640625" customWidth="1"/>
-    <col min="54" max="55" width="0" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="25.6640625" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="25" max="35" width="25.6640625" customWidth="1"/>
+    <col min="36" max="37" width="0" hidden="1" customWidth="1"/>
+    <col min="38" max="39" width="25.6640625" customWidth="1"/>
+    <col min="40" max="40" width="32.6640625" customWidth="1"/>
+    <col min="41" max="41" width="35.6640625" customWidth="1"/>
+    <col min="42" max="42" width="33.6640625" customWidth="1"/>
+    <col min="43" max="43" width="37.6640625" customWidth="1"/>
+    <col min="44" max="44" width="32.6640625" customWidth="1"/>
+    <col min="45" max="45" width="26.6640625" customWidth="1"/>
+    <col min="46" max="46" width="34.6640625" customWidth="1"/>
+    <col min="47" max="47" width="33.6640625" customWidth="1"/>
+    <col min="48" max="56" width="25.6640625" customWidth="1"/>
     <col min="57" max="58" width="0" hidden="1" customWidth="1"/>
     <col min="59" max="59" width="25.6640625" customWidth="1"/>
-    <col min="60" max="60" width="37.6640625" customWidth="1"/>
+    <col min="60" max="61" width="0" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="25.6640625" customWidth="1"/>
+    <col min="63" max="63" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>370</v>
       </c>
@@ -14213,124 +14232,133 @@
         <v>216</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" ht="306" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -14395,109 +14423,109 @@
         <v>78</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>1583</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BC2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="BE2" s="2" t="s">
         <v>74</v>
@@ -14506,13 +14534,22 @@
         <v>78</v>
       </c>
       <c r="BG2" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BK2" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -14571,116 +14608,125 @@
         <v>1498</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>1584</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AN3" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="AM3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2" t="s">
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2" t="s">
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="BA3" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="AY3" s="2" t="s">
+      <c r="BB3" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="AZ3" s="2" t="s">
+      <c r="BC3" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="BA3" s="2" t="s">
+      <c r="BD3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BB3" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="BC3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BD3" s="2" t="s">
+      <c r="BG3" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BH3" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BI3" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="BG3" s="2" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="BH3" s="2" t="s">
+      <c r="BK3" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>371</v>
       </c>
@@ -14745,124 +14791,133 @@
         <v>408</v>
       </c>
       <c r="V4" t="s">
+        <v>1577</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1578</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="Y4" t="s">
         <v>412</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>416</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" t="s">
         <v>420</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>424</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" t="s">
         <v>428</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AD4" t="s">
         <v>432</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AE4" t="s">
         <v>436</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AF4" t="s">
         <v>440</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AG4" t="s">
         <v>444</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
         <v>448</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AI4" t="s">
         <v>450</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
         <v>452</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" t="s">
         <v>454</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AL4" t="s">
         <v>458</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AM4" t="s">
         <v>461</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AN4" t="s">
         <v>465</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AO4" t="s">
         <v>469</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AP4" t="s">
         <v>473</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AQ4" t="s">
         <v>477</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AR4" t="s">
         <v>481</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AS4" t="s">
         <v>485</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AT4" t="s">
         <v>118</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AU4" t="s">
         <v>490</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AV4" t="s">
         <v>321</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AW4" t="s">
         <v>324</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AX4" t="s">
         <v>327</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AY4" t="s">
         <v>331</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AZ4" t="s">
         <v>335</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BA4" t="s">
         <v>339</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BB4" t="s">
         <v>342</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BC4" t="s">
         <v>346</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BD4" t="s">
         <v>348</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BE4" t="s">
         <v>350</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BF4" t="s">
         <v>352</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BG4" t="s">
         <v>356</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BH4" t="s">
         <v>359</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BI4" t="s">
         <v>361</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BJ4" t="s">
         <v>365</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BK4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -14925,6 +14980,9 @@
       <c r="BF5" s="1"/>
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14935,8 +14993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BH5"/>
   <sheetViews>
-    <sheetView topLeftCell="AN2" workbookViewId="0">
-      <selection activeCell="AR6" sqref="AR6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15500,7 +15558,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>492</v>
       </c>

</xml_diff>

<commit_message>
Add hca_bionetwork module to the project tab
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idazucchi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Documents/Schema-change-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB25997-AA76-DB4B-9385-0AD0F9D8E6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29226B4-C33D-DD4C-97F2-69C68950EC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4580" yWindow="-21600" windowWidth="38400" windowHeight="21600" firstSheet="20" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14060" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -43,14 +43,13 @@
     <sheet name="Imaging protocol - Channel" sheetId="25" r:id="rId28"/>
     <sheet name="Imaging protocol - Probe" sheetId="26" r:id="rId29"/>
     <sheet name="Familial relationship" sheetId="27" r:id="rId30"/>
-    <sheet name="Schemas" sheetId="28" r:id="rId31"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3066" uniqueCount="1586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1574">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4327,9 +4326,6 @@
     <t>donor_organism.familial_relationships.sibling</t>
   </si>
   <si>
-    <t>Schemas</t>
-  </si>
-  <si>
     <t>EGA Study/Dataset Accession(s)</t>
   </si>
   <si>
@@ -4624,84 +4620,6 @@
     <t>treatment_protocol.target_pathway.ontology_label</t>
   </si>
   <si>
-    <t>https://schema.humancellatlas.org/type/protocol/sequencing/10.1.0/sequencing_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/sequencing/6.3.1/library_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/imaging/11.4.0/imaging_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/imaging/2.3.0/imaging_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/3.2.0/ipsc_induction_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/3.1.0/enrichment_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/6.2.0/dissociation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.2.0/differentiation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/9.2.0/collection_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.1.0/aggregate_generation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/analysis/9.2.0/analysis_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/7.1.0/protocol</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/project/17.0.0/project</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/process/sequencing/5.1.0/library_preparation_process</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/process/9.2.0/process</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/file/2.5.0/supplementary_file</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/file/9.5.0/sequence_file</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/file/3.5.0/reference_file</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/file/2.5.0/image_file</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/file/6.5.0/analysis_file</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/11.3.0/organoid</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/3.3.0/imaged_specimen</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/15.6.0/donor_organism</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/13.3.0/cell_suspension</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/15.1.0/cell_line</t>
-  </si>
-  <si>
-    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/1.0.0/treatment_protocol</t>
-  </si>
-  <si>
     <t>TREATMENT MEDIA</t>
   </si>
   <si>
@@ -4807,14 +4725,59 @@
     <t>If a healthy specimen is sampled from a site adjacent to diseased tissue, enter that tissue's disease here. If no diseased tissue is adjacent to the specimen, leave blank. For example: type 2 diabetes mellitus; normal; hepatic steatosis</t>
   </si>
   <si>
-    <t>https://schema.humancellatlas.org/type/biomaterial/10.6.0/specimen_from_organism</t>
+    <t>OFFICIAL HCA BIONETWORK</t>
+  </si>
+  <si>
+    <t>HCA Bionetwork the project is a part of (e.g. Kidney).</t>
+  </si>
+  <si>
+    <t>Should be one of the networks from https://www.humancellatlas.org/biological-networks/</t>
+  </si>
+  <si>
+    <t>HCA TISSUE ATLAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A field describing if the project is part of a HCA Tissue Atlas (e.g. Brain Alzheimer Atlas). </t>
+  </si>
+  <si>
+    <t>For example: Blood Atlas</t>
+  </si>
+  <si>
+    <t>OFFICIAL HCA TISSUE ATLAS VERSION</t>
+  </si>
+  <si>
+    <t>A field describing which version of the HCA Tissue Atlas is associated with the project (e.g. v1.0; v2.0)</t>
+  </si>
+  <si>
+    <t>For example: v1.0; v2.0</t>
+  </si>
+  <si>
+    <t>PROJECT TISSUE ATLAS STATUS</t>
+  </si>
+  <si>
+    <t>A field describing if this project is the HCA Tissue Atlas project which integrates data from other datasets.</t>
+  </si>
+  <si>
+    <t>Enter ‘Yes’ if this project is one of the HCA Tissue Atlases and it integrates data from all other datasets. Enter ‘No’, if this project's data is being integrated.</t>
+  </si>
+  <si>
+    <t>project.hca_bionetwork.hca_tissue_atlas</t>
+  </si>
+  <si>
+    <t>project.hca_bionetwork.hca_tissue_atlas_version</t>
+  </si>
+  <si>
+    <t>project.hca_bionetwork.atlas_project</t>
+  </si>
+  <si>
+    <t>project.hca_bionetwork.name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4844,12 +4807,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF24292F"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4891,7 +4848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4907,14 +4864,13 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5255,10 +5211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5269,9 +5225,10 @@
     <col min="10" max="10" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5300,16 +5257,28 @@
         <v>33</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1426</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1427</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="272" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5338,16 +5307,28 @@
         <v>34</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>1428</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>1429</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+        <v>1479</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>1565</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5376,16 +5357,28 @@
         <v>35</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>1431</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>1481</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>1480</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5414,16 +5407,28 @@
         <v>36</v>
       </c>
       <c r="J4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="K4" t="s">
         <v>1432</v>
       </c>
-      <c r="K4" t="s">
-        <v>1433</v>
-      </c>
       <c r="L4" t="s">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1478</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5438,6 +5443,10 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6108,13 +6117,13 @@
         <v>782</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="AU3" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AV3" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>1498</v>
       </c>
       <c r="AW3" s="2" t="s">
         <v>174</v>
@@ -6917,7 +6926,7 @@
         <v>824</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>838</v>
@@ -7012,7 +7021,7 @@
         <v>825</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>839</v>
@@ -7107,7 +7116,7 @@
         <v>826</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>840</v>
@@ -7194,7 +7203,7 @@
         <v>837</v>
       </c>
       <c r="G4" t="s">
-        <v>1564</v>
+        <v>1537</v>
       </c>
       <c r="H4" t="s">
         <v>841</v>
@@ -7899,13 +7908,13 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1502</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1503</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1504</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>92</v>
@@ -7917,16 +7926,16 @@
         <v>885</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>1504</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1505</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1506</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>1507</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>1550</v>
+        <v>1523</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>895</v>
@@ -7947,13 +7956,13 @@
         <v>904</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>1508</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>1509</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>1510</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="68" x14ac:dyDescent="0.2">
@@ -7976,16 +7985,16 @@
         <v>886</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1552</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>1562</v>
-      </c>
-      <c r="I2" s="10" t="s">
+        <v>1525</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>1535</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>78</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1551</v>
+        <v>1524</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>463</v>
@@ -8005,13 +8014,13 @@
       <c r="P2" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>1554</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>1562</v>
-      </c>
-      <c r="S2" s="10" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>1527</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>1535</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -8031,13 +8040,13 @@
         <v>887</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1553</v>
+        <v>1526</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1563</v>
+        <v>1536</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1553</v>
+        <v>1526</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>938</v>
@@ -8061,72 +8070,72 @@
         <v>484</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>1555</v>
+        <v>1528</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1563</v>
+        <v>1536</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>1555</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B4" t="s">
         <v>1511</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1512</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1513</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1514</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1515</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>1516</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>1517</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1518</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>1519</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>1529</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1530</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1532</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1533</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1534</v>
+      </c>
+      <c r="Q4" t="s">
         <v>1520</v>
       </c>
-      <c r="K4" t="s">
-        <v>1556</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1557</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1558</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1559</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1560</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1561</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>1521</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>1522</v>
-      </c>
-      <c r="S4" t="s">
-        <v>1523</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -9873,7 +9882,7 @@
         <v>1151</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="306" x14ac:dyDescent="0.2">
@@ -10182,16 +10191,16 @@
         <v>1176</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>1487</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1488</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1489</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>1490</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>1180</v>
@@ -10512,13 +10521,13 @@
         <v>1178</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>1170</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>1178</v>
@@ -10679,16 +10688,16 @@
         <v>1179</v>
       </c>
       <c r="K4" t="s">
+        <v>1492</v>
+      </c>
+      <c r="L4" t="s">
         <v>1493</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>1494</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>1495</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1496</v>
       </c>
       <c r="O4" t="s">
         <v>1183</v>
@@ -11153,7 +11162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B387E90-E3CD-9746-8D43-32F9BE05CBD7}">
   <dimension ref="A1:AD103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -11198,25 +11207,25 @@
         <v>819</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>824</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1547</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1459</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>1573</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1574</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1460</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>491</v>
@@ -11243,7 +11252,7 @@
         <v>332</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>340</v>
@@ -11258,16 +11267,16 @@
         <v>349</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>1462</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>1463</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>357</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>362</v>
@@ -11284,7 +11293,7 @@
         <v>812</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>74</v>
@@ -11296,16 +11305,16 @@
         <v>825</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1571</v>
+        <v>1544</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1572</v>
+        <v>1545</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>488</v>
@@ -11386,16 +11395,16 @@
         <v>826</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1575</v>
+        <v>1548</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1576</v>
+        <v>1549</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>489</v>
@@ -11446,37 +11455,37 @@
     </row>
     <row r="4" spans="1:30" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B4" t="s">
         <v>1466</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>1467</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" t="s">
         <v>1468</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1469</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1470</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>1476</v>
+      </c>
+      <c r="H4" t="s">
         <v>1471</v>
       </c>
-      <c r="G4" t="s">
-        <v>1477</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1472</v>
-      </c>
       <c r="I4" t="s">
-        <v>1569</v>
+        <v>1542</v>
       </c>
       <c r="J4" t="s">
-        <v>1570</v>
+        <v>1543</v>
       </c>
       <c r="K4" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>492</v>
@@ -11994,13 +12003,13 @@
   <sheetData>
     <row r="1" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1434</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1435</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1436</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>92</v>
@@ -12009,22 +12018,22 @@
         <v>881</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1437</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1438</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1439</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1440</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1441</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1442</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -12048,7 +12057,7 @@
         <v>882</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1565</v>
+        <v>1538</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>74</v>
@@ -12057,13 +12066,13 @@
         <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1567</v>
+        <v>1540</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>1443</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>1444</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -12083,7 +12092,7 @@
         <v>883</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1566</v>
+        <v>1539</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>358</v>
@@ -12092,13 +12101,13 @@
         <v>355</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1568</v>
+        <v>1541</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1445</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>1446</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -12107,37 +12116,37 @@
     </row>
     <row r="4" spans="1:15" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B4" t="s">
         <v>1447</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1448</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1449</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1450</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1451</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>1452</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>1453</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1454</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>1477</v>
+      </c>
+      <c r="K4" t="s">
         <v>1455</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1478</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1456</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -12701,7 +12710,7 @@
         <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
@@ -12721,7 +12730,7 @@
         <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -12741,7 +12750,7 @@
         <v>102</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -12761,7 +12770,7 @@
         <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -12846,167 +12855,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:A28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1425</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>1531</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13048,7 +12902,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -13059,7 +12913,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -13665,13 +13519,13 @@
         <v>204</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="AD3" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>1498</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>220</v>
@@ -14232,13 +14086,13 @@
         <v>216</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1580</v>
+        <v>1553</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1581</v>
+        <v>1554</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1582</v>
+        <v>1555</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>409</v>
@@ -14423,7 +14277,7 @@
         <v>78</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>1583</v>
+        <v>1556</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>74</v>
@@ -14599,22 +14453,22 @@
         <v>403</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>1497</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>1498</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>1584</v>
+        <v>1557</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>1498</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>411</v>
@@ -14791,13 +14645,13 @@
         <v>408</v>
       </c>
       <c r="V4" t="s">
-        <v>1577</v>
+        <v>1550</v>
       </c>
       <c r="W4" t="s">
-        <v>1578</v>
+        <v>1551</v>
       </c>
       <c r="X4" t="s">
-        <v>1579</v>
+        <v>1552</v>
       </c>
       <c r="Y4" t="s">
         <v>412</v>
@@ -15157,7 +15011,7 @@
         <v>599</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>319</v>
@@ -15689,7 +15543,7 @@
         <v>600</v>
       </c>
       <c r="AR4" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="AS4" t="s">
         <v>321</v>

</xml_diff>

<commit_message>
Fix hca_bionetworks property name
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Documents/Schema-change-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29226B4-C33D-DD4C-97F2-69C68950EC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D979D1-9C3C-5245-9FF6-7E1B0AF8EC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -4761,16 +4761,16 @@
     <t>Enter ‘Yes’ if this project is one of the HCA Tissue Atlases and it integrates data from all other datasets. Enter ‘No’, if this project's data is being integrated.</t>
   </si>
   <si>
-    <t>project.hca_bionetwork.hca_tissue_atlas</t>
-  </si>
-  <si>
-    <t>project.hca_bionetwork.hca_tissue_atlas_version</t>
-  </si>
-  <si>
-    <t>project.hca_bionetwork.atlas_project</t>
-  </si>
-  <si>
-    <t>project.hca_bionetwork.name</t>
+    <t>project.hca_bionetworks.name</t>
+  </si>
+  <si>
+    <t>project.hca_bionetworks.hca_tissue_atlas</t>
+  </si>
+  <si>
+    <t>project.hca_bionetworks.hca_tissue_atlas_version</t>
+  </si>
+  <si>
+    <t>project.hca_bionetworks.atlas_project</t>
   </si>
 </sst>
 </file>
@@ -5278,7 +5278,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="272" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5416,16 +5416,16 @@
         <v>1478</v>
       </c>
       <c r="M4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P4" t="s">
         <v>1573</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1570</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add alignment software & version to analysis_protocol
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idazucchi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F98B85-8D9C-024A-BA8F-18687994C95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D871456-7713-ED45-9213-36111E3D072D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" firstSheet="22" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,25 @@
     <sheet name="Imaging protocol - Probe" sheetId="26" r:id="rId29"/>
     <sheet name="Familial relationship" sheetId="27" r:id="rId30"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="1594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="1603">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4831,6 +4844,33 @@
   </si>
   <si>
     <t>cell_line.biomaterial_core.timecourse.relevance</t>
+  </si>
+  <si>
+    <t>analysis_protocol.alignment_software</t>
+  </si>
+  <si>
+    <t>Name of alignment software used to map FASTQ files to reference genome.</t>
+  </si>
+  <si>
+    <t>ALIGNMENT SOFTWARE</t>
+  </si>
+  <si>
+    <t>For example: Cellranger; kallisto bustools; GSNAP; STAR</t>
+  </si>
+  <si>
+    <t>For example: enzymatic dissociation; blood draw</t>
+  </si>
+  <si>
+    <t>ALIGNMENT SOFTWARE VERSION</t>
+  </si>
+  <si>
+    <t>Version of alignment software used to map FASTQ files to reference genome.</t>
+  </si>
+  <si>
+    <t>For example: v2.0.1; 2.4.2a; v0.45.2</t>
+  </si>
+  <si>
+    <t>analysis_protocol.alignment_software_version</t>
   </si>
 </sst>
 </file>
@@ -5239,9 +5279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5304,7 +5342,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5354,7 +5392,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="170" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5404,7 +5442,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5454,7 +5492,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5483,9 +5521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BE5" sqref="BE5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5769,7 +5805,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:81" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:81" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -6014,7 +6050,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:81" ht="170" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:81" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -6245,7 +6281,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:81" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>696</v>
       </c>
@@ -6584,9 +6620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6671,7 +6705,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>798</v>
       </c>
@@ -6742,7 +6776,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>799</v>
       </c>
@@ -6807,7 +6841,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>800</v>
       </c>
@@ -6914,9 +6948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7031,7 +7063,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>798</v>
       </c>
@@ -7126,7 +7158,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>799</v>
       </c>
@@ -7213,7 +7245,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>822</v>
       </c>
@@ -7443,7 +7475,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>798</v>
       </c>
@@ -7517,7 +7549,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>799</v>
       </c>
@@ -7583,7 +7615,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>853</v>
       </c>
@@ -7754,7 +7786,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -7801,7 +7833,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -7844,7 +7876,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>485</v>
       </c>
@@ -7919,9 +7951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2F1E06-C83F-9240-A431-D0EEE8C93825}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7995,7 +8025,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -8054,7 +8084,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -8109,7 +8139,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1500</v>
       </c>
@@ -8260,7 +8290,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -8307,7 +8337,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -8350,7 +8380,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>593</v>
       </c>
@@ -8498,7 +8528,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -8557,7 +8587,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -8612,7 +8642,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>666</v>
       </c>
@@ -8703,9 +8733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8758,7 +8786,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -8796,7 +8824,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -8830,7 +8858,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>595</v>
       </c>
@@ -8931,7 +8959,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -8957,7 +8985,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -8979,7 +9007,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>664</v>
       </c>
@@ -9073,7 +9101,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>38</v>
       </c>
@@ -9111,7 +9139,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -9149,7 +9177,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -9284,7 +9312,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -9337,7 +9365,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -9386,7 +9414,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>796</v>
       </c>
@@ -9566,7 +9594,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -9643,7 +9671,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -9716,7 +9744,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>694</v>
       </c>
@@ -9915,7 +9943,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -9980,7 +10008,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -10041,7 +10069,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>861</v>
       </c>
@@ -10140,9 +10168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10189,7 +10215,7 @@
     <col min="55" max="55" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="4" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>849</v>
       </c>
@@ -10356,7 +10382,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="142" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -10523,7 +10549,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="142" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -10686,7 +10712,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="4" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>850</v>
       </c>
@@ -10921,9 +10947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10997,7 +11021,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -11053,7 +11077,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="221" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -11105,7 +11129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>852</v>
       </c>
@@ -11192,9 +11216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B387E90-E3CD-9746-8D43-32F9BE05CBD7}">
   <dimension ref="A1:AD103"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11223,7 +11245,7 @@
     <col min="31" max="31" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>797</v>
       </c>
@@ -11315,7 +11337,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>798</v>
       </c>
@@ -11407,7 +11429,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>799</v>
       </c>
@@ -11483,7 +11505,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1455</v>
       </c>
@@ -12008,30 +12030,31 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="84.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="17" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="10" width="24.1640625" customWidth="1"/>
+    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.6640625" customWidth="1"/>
+    <col min="13" max="13" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.6640625" customWidth="1"/>
+    <col min="17" max="19" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1423</v>
       </c>
@@ -12057,20 +12080,26 @@
         <v>1428</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>1596</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1599</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1429</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1430</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1431</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -12096,20 +12125,26 @@
         <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>1595</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>1530</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>1433</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -12128,23 +12163,29 @@
         <v>353</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>350</v>
+        <v>1598</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>1597</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1531</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>1434</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>1435</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1436</v>
       </c>
@@ -12170,16 +12211,22 @@
         <v>1443</v>
       </c>
       <c r="I4" t="s">
+        <v>1594</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1602</v>
+      </c>
+      <c r="K4" t="s">
         <v>1444</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>1467</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>1445</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -12197,6 +12244,8 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12234,7 +12283,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>458</v>
       </c>
@@ -12254,7 +12303,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>459</v>
       </c>
@@ -12274,7 +12323,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1319</v>
       </c>
@@ -12347,7 +12396,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1326</v>
       </c>
@@ -12370,7 +12419,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1327</v>
       </c>
@@ -12393,7 +12442,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1328</v>
       </c>
@@ -12436,9 +12485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12512,7 +12559,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1353</v>
       </c>
@@ -12568,7 +12615,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1354</v>
       </c>
@@ -12624,7 +12671,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1355</v>
       </c>
@@ -12711,9 +12758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12743,7 +12788,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -12763,7 +12808,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -12783,7 +12828,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -12840,7 +12885,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1404</v>
       </c>
@@ -12851,7 +12896,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1405</v>
       </c>
@@ -12862,7 +12907,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1406</v>
       </c>
@@ -12889,9 +12934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12910,7 +12953,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>105</v>
       </c>
@@ -12921,7 +12964,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>106</v>
       </c>
@@ -12932,7 +12975,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -12943,7 +12986,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -12959,9 +13002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BY5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BF3" sqref="BF3:BF5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13236,7 +13277,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:77" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:77" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -13469,7 +13510,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:77" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -13690,7 +13731,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:77" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -14013,9 +14054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BP5"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AP4" sqref="AO4:AP4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14261,7 +14300,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:68" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:68" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -14467,7 +14506,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:68" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:68" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -14659,7 +14698,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>366</v>
       </c>
@@ -14946,9 +14985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BM5"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AS4" sqref="AS4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15180,7 +15217,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:65" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:65" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -15377,7 +15414,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="170" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:65" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -15560,7 +15597,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:65" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>487</v>
       </c>
@@ -15835,9 +15872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16036,7 +16071,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -16203,7 +16238,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -16356,7 +16391,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>597</v>
       </c>
@@ -16591,9 +16626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R4" sqref="Q4:R4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16730,7 +16763,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="306" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -16843,7 +16876,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -16942,7 +16975,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>668</v>
       </c>

</xml_diff>

<commit_message>
Add gene_annotation_version to analysis_protocol
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF8F470-D25B-884E-AE9F-0AF65A8CF66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB75E88-1B46-B047-ADC9-D2E3C6E8BE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="5840" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10480" yWindow="5840" windowWidth="30240" windowHeight="17640" firstSheet="19" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="1598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3126" uniqueCount="1602">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4856,6 +4856,18 @@
   </si>
   <si>
     <t>analysis_protocol.alignment_software_version</t>
+  </si>
+  <si>
+    <t>GENE ANNOTATION VERSION</t>
+  </si>
+  <si>
+    <t>analysis_protocol.gene_annotation_version</t>
+  </si>
+  <si>
+    <t>The Ensembl release version accession number or NCBI RefSeq assembly version used for gene annotation.</t>
+  </si>
+  <si>
+    <t>For example: v110; GCF_000001405.40; GCF_000001635.27</t>
   </si>
 </sst>
 </file>
@@ -5264,7 +5276,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12015,10 +12029,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12030,16 +12044,16 @@
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="10" width="24.1640625" customWidth="1"/>
-    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.6640625" customWidth="1"/>
-    <col min="13" max="13" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.6640625" customWidth="1"/>
-    <col min="17" max="19" width="8.83203125" customWidth="1"/>
+    <col min="9" max="11" width="24.1640625" customWidth="1"/>
+    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.6640625" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.6640625" customWidth="1"/>
+    <col min="18" max="20" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1418</v>
       </c>
@@ -12071,20 +12085,23 @@
         <v>1594</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>1598</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>1424</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1425</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1426</v>
       </c>
-      <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -12116,20 +12133,23 @@
         <v>1595</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>1427</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>1428</v>
       </c>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -12157,20 +12177,23 @@
         <v>1596</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>1429</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1431</v>
       </c>
@@ -12202,16 +12225,19 @@
         <v>1597</v>
       </c>
       <c r="K4" t="s">
+        <v>1599</v>
+      </c>
+      <c r="L4" t="s">
         <v>1439</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>1462</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>1440</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -12231,6 +12257,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14970,7 +14997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BH5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AO1:AS1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fix organ_parts typo in programmatic name
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4E7F72-8B31-EF4D-B6F4-7B51A24CBA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695B3EEE-71C4-1842-B21B-C87E304FE7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73940" yWindow="-920" windowWidth="27800" windowHeight="19200" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="1613">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4895,6 +4895,12 @@
   </si>
   <si>
     <t>project.duos_id</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ_parts.ontology</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ_parts.ontology_label</t>
   </si>
 </sst>
 </file>
@@ -14122,7 +14128,7 @@
   <dimension ref="A1:BQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14133,9 +14139,9 @@
     <col min="4" max="10" width="25.6640625" customWidth="1"/>
     <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="25.6640625" customWidth="1"/>
-    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="8.83203125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="25.6640625" customWidth="1"/>
-    <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="18" width="8.83203125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.6640625" customWidth="1"/>
     <col min="21" max="22" width="8.83203125" hidden="1" customWidth="1"/>
@@ -14827,10 +14833,10 @@
         <v>393</v>
       </c>
       <c r="Q4" t="s">
-        <v>393</v>
+        <v>1611</v>
       </c>
       <c r="R4" t="s">
-        <v>393</v>
+        <v>1612</v>
       </c>
       <c r="S4" t="s">
         <v>1606</v>

</xml_diff>

<commit_message>
Fix typo in intron_inclusion programmatic name
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A82185-A5DC-9E4D-AFC3-4B4E284977F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDF862B-7D5E-9542-B232-215D51F50A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="77600" yWindow="-1240" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" firstSheet="24" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="1616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="1617">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4910,6 +4910,9 @@
   </si>
   <si>
     <t>Should be one of: yes, or no.</t>
+  </si>
+  <si>
+    <t>analysis_protocol.intron_inclusion</t>
   </si>
 </sst>
 </file>
@@ -5318,7 +5321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12104,7 +12107,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D194D221-20CF-2E41-90C4-A993C89EE7F6}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12308,7 +12313,7 @@
         <v>1597</v>
       </c>
       <c r="L4" t="s">
-        <v>1597</v>
+        <v>1616</v>
       </c>
       <c r="M4" t="s">
         <v>1437</v>
@@ -14150,7 +14155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BQ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BQ1" sqref="BQ1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Add Schema tab in hca_template.xlsx
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B38024-950B-5D43-92C6-E7114FA6F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CD17B4-D125-CD49-8C74-AEDDC3AD6C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="5860" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="29560" windowWidth="21360" windowHeight="17600" firstSheet="25" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,7 @@
     <sheet name="Imaging protocol - Channel" sheetId="25" r:id="rId28"/>
     <sheet name="Imaging protocol - Probe" sheetId="26" r:id="rId29"/>
     <sheet name="Familial relationship" sheetId="27" r:id="rId30"/>
+    <sheet name="Schemas" sheetId="32" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="1630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3191" uniqueCount="1665">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4952,13 +4953,118 @@
   </si>
   <si>
     <t>Should be of the networks from https://www.humancellatlas.org/biological-networks/</t>
+  </si>
+  <si>
+    <t>Schemas</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/2.5.0/image_file</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/7.0.0/analysis_file</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/9.2.0/collection_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/imaging/2.3.0/imaging_preparation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/9.2.0/process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/10.9.0/specimen_from_organism</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/3.5.0/imaged_specimen</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/14.0.0/cell_suspension</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/imaging/11.4.0/imaging_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/sequencing/6.3.1/library_preparation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/9.6.0/sequence_file</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/6.2.0/dissociation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/sequencing/10.1.0/sequencing_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/analysis/10.3.0/analysis_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/1.0.0/treatment_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/3.2.0/ipsc_induction_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/3.1.0/enrichment_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.2.0/differentiation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.1.0/aggregate_generation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial/5.1.0/biomaterial_collection_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/7.1.0/protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/project/19.0.1/project</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/sequencing/5.1.0/sequencing_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/sequencing/5.1.0/library_preparation_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/imaging/5.1.0/imaging_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/enrichment_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/dissociation_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/collection_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/analysis/12.0.0/analysis_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/11.5.0/organoid</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/16.3.0/donor_organism</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/16.0.0/cell_line</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/module/project/1.0.2/hca_bionetwork</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/2.5.0/supplementary_file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5009,6 +5115,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5037,7 +5149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5069,6 +5181,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5376,7 +5489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13134,6 +13247,196 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C18686-9D1F-1749-B0F4-D3AC8CBFF263}">
+  <dimension ref="A1:A35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>

</xml_diff>

<commit_message>
Remove function in hca_template.xlsx
</commit_message>
<xml_diff>
--- a/template/hca_template.xlsx
+++ b/template/hca_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC7EF56-9586-BA4A-9A13-50ECEC29F1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666C9DB1-1D45-3A4E-94E8-9D6D0C5E3947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80220" yWindow="-1100" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="77160" yWindow="180" windowWidth="21360" windowHeight="17600" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="1684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="1684">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -5556,7 +5556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9370,7 +9370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9434,9 +9436,8 @@
       <c r="O1" s="3" t="s">
         <v>1668</v>
       </c>
-      <c r="P1" s="1" t="str">
-        <f>UPPER("Purchased reagents - RETAIL NAME")</f>
-        <v>PURCHASED REAGENTS - RETAIL NAME</v>
+      <c r="P1" s="1" t="s">
+        <v>869</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>695</v>

</xml_diff>